<commit_message>
pushing all coded indicators
</commit_message>
<xml_diff>
--- a/input/tool/REACH_SOM_DSA_Survey_Tool_v7.xlsx
+++ b/input/tool/REACH_SOM_DSA_Survey_Tool_v7.xlsx
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">settings!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$AB$424</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -8880,7 +8880,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -8953,6 +8953,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9248,8 +9250,8 @@
   <dimension ref="A1:AE424"/>
   <sheetViews>
     <sheetView zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B304" sqref="B304"/>
+      <pane ySplit="1" topLeftCell="A320" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C326" sqref="C326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21941,8 +21943,8 @@
   <dimension ref="A1:I839"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A604" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B601" sqref="B601"/>
+      <pane ySplit="1" topLeftCell="A659" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C670" sqref="C670"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29008,10 +29010,10 @@
       <c r="B409" t="s">
         <v>2391</v>
       </c>
-      <c r="C409" t="s">
+      <c r="C409" s="38" t="s">
         <v>1631</v>
       </c>
-      <c r="D409" t="s">
+      <c r="D409" s="38" t="s">
         <v>1632</v>
       </c>
       <c r="E409" t="s">
@@ -29025,10 +29027,10 @@
       <c r="B410" t="s">
         <v>2391</v>
       </c>
-      <c r="C410" t="s">
+      <c r="C410" s="39" t="s">
         <v>1634</v>
       </c>
-      <c r="D410" t="s">
+      <c r="D410" s="39" t="s">
         <v>1635</v>
       </c>
       <c r="E410" t="s">
@@ -29042,10 +29044,10 @@
       <c r="B411" t="s">
         <v>2391</v>
       </c>
-      <c r="C411" t="s">
+      <c r="C411" s="38" t="s">
         <v>1637</v>
       </c>
-      <c r="D411" t="s">
+      <c r="D411" s="38" t="s">
         <v>1638</v>
       </c>
       <c r="E411" t="s">
@@ -29059,10 +29061,10 @@
       <c r="B412" t="s">
         <v>2391</v>
       </c>
-      <c r="C412" t="s">
+      <c r="C412" s="39" t="s">
         <v>1639</v>
       </c>
-      <c r="D412" t="s">
+      <c r="D412" s="39" t="s">
         <v>1640</v>
       </c>
       <c r="E412" t="s">
@@ -29076,10 +29078,10 @@
       <c r="B413" t="s">
         <v>2391</v>
       </c>
-      <c r="C413" t="s">
+      <c r="C413" s="38" t="s">
         <v>1642</v>
       </c>
-      <c r="D413" s="13" t="s">
+      <c r="D413" s="40" t="s">
         <v>1643</v>
       </c>
       <c r="E413" t="s">
@@ -29093,10 +29095,10 @@
       <c r="B414" t="s">
         <v>2391</v>
       </c>
-      <c r="C414" t="s">
+      <c r="C414" s="39" t="s">
         <v>1644</v>
       </c>
-      <c r="D414" s="13" t="s">
+      <c r="D414" s="41" t="s">
         <v>2420</v>
       </c>
       <c r="E414" t="s">
@@ -29110,10 +29112,10 @@
       <c r="B415" t="s">
         <v>2391</v>
       </c>
-      <c r="C415" t="s">
+      <c r="C415" s="39" t="s">
         <v>1645</v>
       </c>
-      <c r="D415" s="13" t="s">
+      <c r="D415" s="41" t="s">
         <v>2421</v>
       </c>
       <c r="E415" t="s">
@@ -29127,10 +29129,10 @@
       <c r="B416" t="s">
         <v>2391</v>
       </c>
-      <c r="C416" t="s">
+      <c r="C416" s="39" t="s">
         <v>1646</v>
       </c>
-      <c r="D416" s="13" t="s">
+      <c r="D416" s="41" t="s">
         <v>2422</v>
       </c>
       <c r="E416" t="s">
@@ -29144,10 +29146,10 @@
       <c r="B417" t="s">
         <v>2391</v>
       </c>
-      <c r="C417" t="s">
+      <c r="C417" s="39" t="s">
         <v>1647</v>
       </c>
-      <c r="D417" s="13" t="s">
+      <c r="D417" s="41" t="s">
         <v>2423</v>
       </c>
       <c r="E417" t="s">
@@ -29161,10 +29163,10 @@
       <c r="B418" t="s">
         <v>2391</v>
       </c>
-      <c r="C418" t="s">
+      <c r="C418" s="38" t="s">
         <v>1648</v>
       </c>
-      <c r="D418" s="13" t="s">
+      <c r="D418" s="40" t="s">
         <v>2424</v>
       </c>
       <c r="E418" t="s">
@@ -33132,10 +33134,10 @@
       <c r="B665" t="s">
         <v>2403</v>
       </c>
-      <c r="C665" t="s">
+      <c r="C665" s="39" t="s">
         <v>2125</v>
       </c>
-      <c r="D665" t="s">
+      <c r="D665" s="39" t="s">
         <v>2126</v>
       </c>
       <c r="E665" t="s">
@@ -33149,10 +33151,10 @@
       <c r="B666" t="s">
         <v>2403</v>
       </c>
-      <c r="C666" t="s">
+      <c r="C666" s="39" t="s">
         <v>2128</v>
       </c>
-      <c r="D666" t="s">
+      <c r="D666" s="39" t="s">
         <v>2129</v>
       </c>
       <c r="E666" t="s">
@@ -33166,10 +33168,10 @@
       <c r="B667" t="s">
         <v>2403</v>
       </c>
-      <c r="C667" t="s">
+      <c r="C667" s="39" t="s">
         <v>2130</v>
       </c>
-      <c r="D667" t="s">
+      <c r="D667" s="39" t="s">
         <v>2131</v>
       </c>
       <c r="E667" t="s">
@@ -33183,10 +33185,10 @@
       <c r="B668" t="s">
         <v>2403</v>
       </c>
-      <c r="C668" t="s">
+      <c r="C668" s="39" t="s">
         <v>2133</v>
       </c>
-      <c r="D668" t="s">
+      <c r="D668" s="39" t="s">
         <v>2134</v>
       </c>
       <c r="E668" t="s">
@@ -33200,10 +33202,10 @@
       <c r="B669" t="s">
         <v>2403</v>
       </c>
-      <c r="C669" t="s">
+      <c r="C669" s="39" t="s">
         <v>2136</v>
       </c>
-      <c r="D669" t="s">
+      <c r="D669" s="39" t="s">
         <v>2137</v>
       </c>
       <c r="E669" t="s">
@@ -33217,10 +33219,10 @@
       <c r="B670" t="s">
         <v>2403</v>
       </c>
-      <c r="C670" t="s">
+      <c r="C670" s="39" t="s">
         <v>2139</v>
       </c>
-      <c r="D670" t="s">
+      <c r="D670" s="39" t="s">
         <v>2140</v>
       </c>
       <c r="E670" t="s">
@@ -33234,10 +33236,10 @@
       <c r="B671" t="s">
         <v>2403</v>
       </c>
-      <c r="C671" t="s">
+      <c r="C671" s="39" t="s">
         <v>2142</v>
       </c>
-      <c r="D671" t="s">
+      <c r="D671" s="39" t="s">
         <v>2143</v>
       </c>
       <c r="E671" t="s">
@@ -33251,10 +33253,10 @@
       <c r="B672" t="s">
         <v>2403</v>
       </c>
-      <c r="C672" t="s">
+      <c r="C672" s="39" t="s">
         <v>2145</v>
       </c>
-      <c r="D672" t="s">
+      <c r="D672" s="39" t="s">
         <v>2146</v>
       </c>
       <c r="E672" t="s">
@@ -33268,10 +33270,10 @@
       <c r="B673" t="s">
         <v>2403</v>
       </c>
-      <c r="C673" t="s">
+      <c r="C673" s="39" t="s">
         <v>2148</v>
       </c>
-      <c r="D673" t="s">
+      <c r="D673" s="39" t="s">
         <v>2149</v>
       </c>
       <c r="E673" t="s">
@@ -33285,10 +33287,10 @@
       <c r="B674" t="s">
         <v>2403</v>
       </c>
-      <c r="C674" t="s">
+      <c r="C674" s="39" t="s">
         <v>2150</v>
       </c>
-      <c r="D674" t="s">
+      <c r="D674" s="39" t="s">
         <v>2151</v>
       </c>
       <c r="E674" t="s">
@@ -33302,10 +33304,10 @@
       <c r="B675" t="s">
         <v>2403</v>
       </c>
-      <c r="C675" t="s">
+      <c r="C675" s="39" t="s">
         <v>2152</v>
       </c>
-      <c r="D675" t="s">
+      <c r="D675" s="39" t="s">
         <v>2153</v>
       </c>
       <c r="E675" t="s">
@@ -33319,10 +33321,10 @@
       <c r="B676" t="s">
         <v>2403</v>
       </c>
-      <c r="C676" t="s">
+      <c r="C676" s="39" t="s">
         <v>2155</v>
       </c>
-      <c r="D676" t="s">
+      <c r="D676" s="39" t="s">
         <v>2156</v>
       </c>
       <c r="E676" t="s">
@@ -33336,10 +33338,10 @@
       <c r="B677" t="s">
         <v>2403</v>
       </c>
-      <c r="C677" t="s">
+      <c r="C677" s="39" t="s">
         <v>2157</v>
       </c>
-      <c r="D677" t="s">
+      <c r="D677" s="39" t="s">
         <v>2158</v>
       </c>
       <c r="E677" t="s">
@@ -33353,10 +33355,10 @@
       <c r="B678" t="s">
         <v>2403</v>
       </c>
-      <c r="C678" t="s">
+      <c r="C678" s="39" t="s">
         <v>2159</v>
       </c>
-      <c r="D678" t="s">
+      <c r="D678" s="39" t="s">
         <v>2160</v>
       </c>
       <c r="E678" t="s">
@@ -33370,10 +33372,10 @@
       <c r="B679" t="s">
         <v>2403</v>
       </c>
-      <c r="C679" t="s">
+      <c r="C679" s="39" t="s">
         <v>2162</v>
       </c>
-      <c r="D679" t="s">
+      <c r="D679" s="39" t="s">
         <v>2163</v>
       </c>
       <c r="E679" t="s">
@@ -33387,10 +33389,10 @@
       <c r="B680" t="s">
         <v>2403</v>
       </c>
-      <c r="C680" t="s">
+      <c r="C680" s="39" t="s">
         <v>2164</v>
       </c>
-      <c r="D680" t="s">
+      <c r="D680" s="39" t="s">
         <v>2165</v>
       </c>
       <c r="E680" t="s">

</xml_diff>

<commit_message>
LSGs And Results table
</commit_message>
<xml_diff>
--- a/input/tool/REACH_SOM_DSA_Survey_Tool_v7.xlsx
+++ b/input/tool/REACH_SOM_DSA_Survey_Tool_v7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/assil_benamor_reach-initiative_org/Documents/DSA 2021/SOM2103_DSA_21/input/tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_1D7969E1AA86C31E290A98B8C4D3ED57592CEB73" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFE67C2C-5F08-8344-BFF3-C3527493D04D}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_1D7969E1AA86C31E290A98B8C4D3ED57592CEB73" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{635544C8-D06C-9A44-8F91-5981A68B5EBE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="760" windowWidth="29240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -9246,9 +9246,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C386" sqref="C386"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C142" sqref="C142:C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>